<commit_message>
feat: agregar panel de tasas de referencia desde fuentes externas
- Crear endpoint /api/rates/reference para obtener tasas del dÃ­a
- Integrar dolar.wilkinsonpc.com.co para USDâ†’COP (TRM y SPOT)
- Agregar EURâ†’USD y GBPâ†’USD desde ExchangeRate-API
- Crear componente ReferenceRatesPanel con diseÃ±o Apple
- Reemplazar tabla 'Tasas vigentes' con panel de referencia
- Mostrar valores de referencia para personalizaciÃ³n de tasas
</commit_message>
<xml_diff>
--- a/Calculadora modelosv1.xlsx
+++ b/Calculadora modelosv1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camca\OneDrive\Documentos\backup\Backup_Sistema_Final_20250920_235900\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBA0CC2-5E7D-4C73-90E2-5FD7F2EDA7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B9154A-3179-4207-A045-2A4C55FDDA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A0BF7857-9429-4B6B-B453-042B72051C53}"/>
   </bookViews>
@@ -542,6 +542,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -550,174 +590,26 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -756,8 +648,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -774,50 +664,160 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF483C07-E410-4489-8F3A-D86B366D7CB6}">
   <dimension ref="B1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,32 +1198,32 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
     </row>
     <row r="3" spans="2:17" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="72" t="s">
+      <c r="D3" s="71"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="74"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="42"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
@@ -1235,99 +1235,99 @@
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="77"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="45"/>
       <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="93"/>
-      <c r="C5" s="94">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15">
         <v>4094</v>
       </c>
-      <c r="D5" s="96">
+      <c r="D5" s="17">
         <v>1.01</v>
       </c>
-      <c r="E5" s="98">
+      <c r="E5" s="19">
         <v>1.2</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="77"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="93"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="80"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="93"/>
+      <c r="F7" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="20" t="s">
+      <c r="G7" s="93"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="21"/>
+      <c r="K7" s="97"/>
     </row>
     <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="99"/>
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="27">
-        <v>0</v>
-      </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="33">
+      <c r="D9" s="100">
+        <v>0</v>
+      </c>
+      <c r="E9" s="101"/>
+      <c r="F9" s="69">
         <f>D9*0.6</f>
         <v>0</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="91">
+      <c r="G9" s="70"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="33">
         <f>(F9*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K9" s="92"/>
+      <c r="K9" s="34"/>
       <c r="M9" s="12"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -1338,22 +1338,22 @@
       <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="35">
+      <c r="D10" s="102">
+        <v>0</v>
+      </c>
+      <c r="E10" s="103"/>
+      <c r="F10" s="65">
         <f>(D10*D5)*0.78</f>
         <v>0</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="81">
+      <c r="G10" s="66"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="27">
         <f>(F10*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K10" s="82"/>
+      <c r="K10" s="28"/>
       <c r="M10" s="12"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
@@ -1364,22 +1364,22 @@
       <c r="C11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="31">
-        <v>0</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="35">
+      <c r="D11" s="104">
+        <v>0</v>
+      </c>
+      <c r="E11" s="105"/>
+      <c r="F11" s="65">
         <f>D11*0.75</f>
         <v>0</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="81">
+      <c r="G11" s="66"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="27">
         <f>(F11*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K11" s="82"/>
+      <c r="K11" s="28"/>
       <c r="M11" s="12"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
@@ -1390,22 +1390,22 @@
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="31">
-        <v>0</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="35">
+      <c r="D12" s="104">
+        <v>0</v>
+      </c>
+      <c r="E12" s="105"/>
+      <c r="F12" s="65">
         <f>D12*0.75</f>
         <v>0</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="81">
+      <c r="G12" s="66"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="27">
         <f>(F12*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K12" s="82"/>
+      <c r="K12" s="28"/>
       <c r="M12" s="12"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
@@ -1416,22 +1416,22 @@
       <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="31">
-        <v>0</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="35">
+      <c r="D13" s="104">
+        <v>0</v>
+      </c>
+      <c r="E13" s="105"/>
+      <c r="F13" s="65">
         <f>D13*0.75</f>
         <v>0</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="81">
+      <c r="G13" s="66"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="27">
         <f>(F13*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K13" s="82"/>
+      <c r="K13" s="28"/>
       <c r="M13" s="12"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
@@ -1442,65 +1442,65 @@
       <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="56">
-        <v>0</v>
-      </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="35">
+      <c r="D14" s="86">
+        <v>0</v>
+      </c>
+      <c r="E14" s="87"/>
+      <c r="F14" s="65">
         <f>D14*0.05</f>
         <v>0</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="81">
+      <c r="G14" s="66"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="27">
         <f>(F14*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="82"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="56">
-        <v>0</v>
-      </c>
-      <c r="E15" s="57"/>
-      <c r="F15" s="35">
+      <c r="D15" s="86">
+        <v>0</v>
+      </c>
+      <c r="E15" s="87"/>
+      <c r="F15" s="65">
         <f>D15*0.05</f>
         <v>0</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="81">
+      <c r="G15" s="66"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="27">
         <f>(F15*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K15" s="82"/>
+      <c r="K15" s="28"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="56">
-        <v>0</v>
-      </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="35">
+      <c r="D16" s="86">
+        <v>0</v>
+      </c>
+      <c r="E16" s="87"/>
+      <c r="F16" s="65">
         <f>D16*0.05</f>
         <v>0</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="81">
+      <c r="G16" s="66"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="27">
         <f>(F16*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K16" s="82"/>
+      <c r="K16" s="28"/>
       <c r="M16" s="12"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
@@ -1510,22 +1510,22 @@
       <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="58">
-        <v>0</v>
-      </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="35">
+      <c r="D17" s="88">
+        <v>0</v>
+      </c>
+      <c r="E17" s="89"/>
+      <c r="F17" s="65">
         <f>D17*D5</f>
         <v>0</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="81">
+      <c r="G17" s="66"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="27">
         <f>(F17*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K17" s="82"/>
+      <c r="K17" s="28"/>
       <c r="M17" s="12"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
@@ -1535,43 +1535,43 @@
       <c r="C18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="60">
-        <v>0</v>
-      </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="35">
+      <c r="D18" s="90">
+        <v>0</v>
+      </c>
+      <c r="E18" s="91"/>
+      <c r="F18" s="65">
         <f>D18</f>
         <v>0</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="81">
+      <c r="G18" s="66"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="27">
         <f>(F18*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K18" s="82"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="54">
-        <v>0</v>
-      </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="35">
+      <c r="D19" s="84">
+        <v>0</v>
+      </c>
+      <c r="E19" s="85"/>
+      <c r="F19" s="65">
         <f>D19*0.5</f>
         <v>0</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="81">
+      <c r="G19" s="66"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="27">
         <f>(F19*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K19" s="82"/>
+      <c r="K19" s="28"/>
       <c r="M19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1580,401 +1580,516 @@
       <c r="C20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="46">
-        <v>0</v>
-      </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="35">
+      <c r="D20" s="78">
+        <v>0</v>
+      </c>
+      <c r="E20" s="79"/>
+      <c r="F20" s="65">
         <f>D20</f>
         <v>0</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="81">
+      <c r="G20" s="66"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="27">
         <f>(F20*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K20" s="82"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="48">
-        <v>0</v>
-      </c>
-      <c r="E21" s="49"/>
-      <c r="F21" s="35">
+      <c r="D21" s="61">
+        <v>0</v>
+      </c>
+      <c r="E21" s="62"/>
+      <c r="F21" s="65">
         <f>D21*D5</f>
         <v>0</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="81">
+      <c r="G21" s="66"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="27">
         <f>(F21*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K21" s="82"/>
+      <c r="K21" s="28"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C22" s="8">
         <v>777</v>
       </c>
-      <c r="D22" s="50">
-        <v>0</v>
-      </c>
-      <c r="E22" s="51"/>
-      <c r="F22" s="35">
+      <c r="D22" s="80">
+        <v>0</v>
+      </c>
+      <c r="E22" s="81"/>
+      <c r="F22" s="65">
         <f>D22*D5</f>
         <v>0</v>
       </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="81">
+      <c r="G22" s="66"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="27">
         <f>(F22*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K22" s="82"/>
+      <c r="K22" s="28"/>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="50">
-        <v>0</v>
-      </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="35">
+      <c r="D23" s="80">
+        <v>0</v>
+      </c>
+      <c r="E23" s="81"/>
+      <c r="F23" s="65">
         <f>D23*D5</f>
         <v>0</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="81">
+      <c r="G23" s="66"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="27">
         <f>(F23*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K23" s="82"/>
+      <c r="K23" s="28"/>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="50">
-        <v>0</v>
-      </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="35">
+      <c r="D24" s="80">
+        <v>0</v>
+      </c>
+      <c r="E24" s="81"/>
+      <c r="F24" s="65">
         <f>D24*D5</f>
         <v>0</v>
       </c>
-      <c r="G24" s="36"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="81">
+      <c r="G24" s="66"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="27">
         <f>(F24*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K24" s="82"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C25" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="52">
-        <v>0</v>
-      </c>
-      <c r="E25" s="53"/>
-      <c r="F25" s="35">
+      <c r="D25" s="82">
+        <v>0</v>
+      </c>
+      <c r="E25" s="83"/>
+      <c r="F25" s="65">
         <f>(D25*E5)*0.677</f>
         <v>0</v>
       </c>
-      <c r="G25" s="36"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="81">
+      <c r="G25" s="66"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="27">
         <f>(F25*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K25" s="82"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="50">
-        <v>0</v>
-      </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="35">
+      <c r="D26" s="80">
+        <v>0</v>
+      </c>
+      <c r="E26" s="81"/>
+      <c r="F26" s="65">
         <f>D26*D5</f>
         <v>0</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="81">
+      <c r="G26" s="66"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="27">
         <f>F26*C5</f>
         <v>0</v>
       </c>
-      <c r="K26" s="82"/>
+      <c r="K26" s="28"/>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="54">
-        <v>0</v>
-      </c>
-      <c r="E27" s="55"/>
-      <c r="F27" s="35">
+      <c r="D27" s="84">
+        <v>0</v>
+      </c>
+      <c r="E27" s="85"/>
+      <c r="F27" s="65">
         <f>D27</f>
         <v>0</v>
       </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="81">
+      <c r="G27" s="66"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="27">
         <f>(F27*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K27" s="82"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="54">
-        <v>0</v>
-      </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="35">
+      <c r="D28" s="84">
+        <v>0</v>
+      </c>
+      <c r="E28" s="85"/>
+      <c r="F28" s="65">
         <f>D28</f>
         <v>0</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="81">
+      <c r="G28" s="66"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="27">
         <f>(F28*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K28" s="82"/>
+      <c r="K28" s="28"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C29" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="40">
-        <v>0</v>
-      </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="35">
+      <c r="D29" s="74">
+        <v>0</v>
+      </c>
+      <c r="E29" s="75"/>
+      <c r="F29" s="65">
         <f>D29</f>
         <v>0</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="81">
+      <c r="G29" s="66"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="27">
         <f>(F29*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K29" s="82"/>
+      <c r="K29" s="28"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C30" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="42">
-        <v>0</v>
-      </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="35">
+      <c r="D30" s="63">
+        <v>0</v>
+      </c>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65">
         <f>D30</f>
         <v>0</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="81">
+      <c r="G30" s="66"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="27">
         <f>(F30*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K30" s="82"/>
+      <c r="K30" s="28"/>
     </row>
     <row r="31" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="44">
-        <v>0</v>
-      </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="62">
+      <c r="D31" s="76">
+        <v>0</v>
+      </c>
+      <c r="E31" s="77"/>
+      <c r="F31" s="67">
         <f>D31*D5</f>
         <v>0</v>
       </c>
-      <c r="G31" s="63"/>
-      <c r="H31" s="104"/>
-      <c r="I31" s="105"/>
-      <c r="J31" s="83">
+      <c r="G31" s="68"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="49">
         <f>(F31*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K31" s="84"/>
+      <c r="K31" s="50"/>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C32" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="70">
-        <v>0</v>
-      </c>
-      <c r="E32" s="71"/>
-      <c r="F32" s="33">
+      <c r="D32" s="59">
+        <v>0</v>
+      </c>
+      <c r="E32" s="60"/>
+      <c r="F32" s="69">
         <f>D32*E5</f>
         <v>0</v>
       </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="91">
+      <c r="G32" s="70"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="33">
         <f>(F32*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K32" s="92"/>
+      <c r="K32" s="34"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C33" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="48">
-        <v>0</v>
-      </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="35">
+      <c r="D33" s="61">
+        <v>0</v>
+      </c>
+      <c r="E33" s="62"/>
+      <c r="F33" s="65">
         <f>(D33*D5)*(1-16%)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="81">
+      <c r="G33" s="66"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="27">
         <f>(F33*C5)*0.6</f>
         <v>0</v>
       </c>
-      <c r="K33" s="82"/>
+      <c r="K33" s="28"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C34" s="8"/>
-      <c r="D34" s="42">
-        <v>0</v>
-      </c>
-      <c r="E34" s="43"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="82"/>
+      <c r="D34" s="63">
+        <v>0</v>
+      </c>
+      <c r="E34" s="64"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C35" s="8"/>
-      <c r="D35" s="42">
-        <v>0</v>
-      </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="82"/>
+      <c r="D35" s="63">
+        <v>0</v>
+      </c>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C36" s="8"/>
-      <c r="D36" s="42">
-        <v>0</v>
-      </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="82"/>
+      <c r="D36" s="63">
+        <v>0</v>
+      </c>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="28"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C37" s="8"/>
-      <c r="D37" s="42">
-        <v>0</v>
-      </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="82"/>
+      <c r="D37" s="63">
+        <v>0</v>
+      </c>
+      <c r="E37" s="64"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
     </row>
     <row r="38" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C38" s="9"/>
-      <c r="D38" s="66">
-        <v>0</v>
-      </c>
-      <c r="E38" s="67"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="104"/>
-      <c r="I38" s="105"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="84"/>
+      <c r="D38" s="57">
+        <v>0</v>
+      </c>
+      <c r="E38" s="58"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="50"/>
     </row>
     <row r="39" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="85">
+      <c r="D39" s="38"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="51">
         <f>SUM(F9:F38)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="86"/>
-      <c r="H39" s="87"/>
-      <c r="I39" s="88"/>
-      <c r="J39" s="89">
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="55">
         <f>SUM(J9:J38)</f>
         <v>0</v>
       </c>
-      <c r="K39" s="90"/>
+      <c r="K39" s="56"/>
     </row>
     <row r="40" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="100" t="s">
+      <c r="F40" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="101"/>
-      <c r="H40" s="101"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
       <c r="I40" s="11">
         <v>0.9</v>
       </c>
-      <c r="J40" s="102">
+      <c r="J40" s="23">
         <f>J39*0.9</f>
         <v>0</v>
       </c>
-      <c r="K40" s="103"/>
+      <c r="K40" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="139">
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="F3:K6"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
@@ -1999,121 +2114,6 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="H32:I32"/>
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="F3:K6"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <conditionalFormatting sqref="F39:G39">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">

</xml_diff>